<commit_message>
Refactor code to split and rename columns in foldchange_df_ix
</commit_message>
<xml_diff>
--- a/TN042/foldchange_ix.xlsx
+++ b/TN042/foldchange_ix.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -444,6 +444,11 @@
           <t>Fold Change</t>
         </is>
       </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>dox</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -451,11 +456,16 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>dusp11 -dox foldchange</t>
+          <t>dusp11</t>
         </is>
       </c>
       <c r="C2" t="n">
         <v>0.4951257660418741</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>-dox</t>
+        </is>
       </c>
     </row>
     <row r="3">
@@ -464,11 +474,16 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>ifnb -dox foldchange</t>
+          <t>ifnb</t>
         </is>
       </c>
       <c r="C3" t="n">
         <v>0.2990535882639475</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>-dox</t>
+        </is>
       </c>
     </row>
     <row r="4">
@@ -477,11 +492,16 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>mx1 -dox foldchange</t>
+          <t>mx1</t>
         </is>
       </c>
       <c r="C4" t="n">
         <v>0.6825846768843439</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>-dox</t>
+        </is>
       </c>
     </row>
     <row r="5">
@@ -490,11 +510,16 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>dusp11 +dox foldchange</t>
+          <t>dusp11</t>
         </is>
       </c>
       <c r="C5" t="n">
         <v>0.3458615801392663</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>+dox</t>
+        </is>
       </c>
     </row>
     <row r="6">
@@ -503,11 +528,16 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>ifnb +dox foldchange</t>
+          <t>ifnb</t>
         </is>
       </c>
       <c r="C6" t="n">
         <v>1.552836929124044</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>+dox</t>
+        </is>
       </c>
     </row>
     <row r="7">
@@ -516,11 +546,16 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>mx1 +dox foldchange</t>
+          <t>mx1</t>
         </is>
       </c>
       <c r="C7" t="n">
         <v>1.214498745700118</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>+dox</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>